<commit_message>
Updated Master Data list for IDA
</commit_message>
<xml_diff>
--- a/requirements/MOSIP Masterdata Types.xlsx
+++ b/requirements/MOSIP Masterdata Types.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CEAAB565-6B5D-42E4-8EA1-12A0961BCC0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Registration" sheetId="8" r:id="rId1"/>
@@ -126,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +149,15 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -233,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -250,6 +260,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1107,52 +1124,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table18" displayName="Table18" ref="B2:E14" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B2:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table18" displayName="Table18" ref="B2:E14" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="B2:E14" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sr No." dataDxfId="27"/>
-    <tableColumn id="2" name="Master Data Type" dataDxfId="26"/>
-    <tableColumn id="3" name="Type" dataDxfId="25"/>
-    <tableColumn id="8" name="Approval Reuiqred for Updation/Deletion" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sr No." dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Master Data Type" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Approval Reuiqred for Updation/Deletion" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B2:E21" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="B2:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table14" displayName="Table14" ref="B2:E21" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B2:E21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sr No." dataDxfId="19"/>
-    <tableColumn id="2" name="Master Data Type" dataDxfId="18"/>
-    <tableColumn id="3" name="Type" dataDxfId="17"/>
-    <tableColumn id="8" name="Approval Reuiqred for Updation/Deletion" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Sr No." dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Master Data Type" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Approval Reuiqred for Updation/Deletion" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="B2:E8" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="B2:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table15" displayName="Table15" ref="B2:E8" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="B2:E8" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sr No." dataDxfId="11"/>
-    <tableColumn id="2" name="Master Data Type" dataDxfId="10"/>
-    <tableColumn id="3" name="Type" dataDxfId="9"/>
-    <tableColumn id="8" name="Approval Reuiqred for Updation/Deletion" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sr No." dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Master Data Type" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Approval Reuiqred for Updation/Deletion" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B2:E13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B2:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table16" displayName="Table16" ref="B2:E13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B2:E13" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Sr No." dataDxfId="3"/>
-    <tableColumn id="2" name="Master Data Type" dataDxfId="2"/>
-    <tableColumn id="3" name="Type" dataDxfId="1"/>
-    <tableColumn id="8" name="Approval Reuiqred for Updation/Deletion" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sr No." dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Master Data Type" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Type" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Approval Reuiqred for Updation/Deletion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1420,23 +1437,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1467,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1464,7 +1481,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1478,7 +1495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1492,7 +1509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1506,7 +1523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1520,7 +1537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1534,7 +1551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1548,7 +1565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1562,7 +1579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1576,7 +1593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1590,7 +1607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1604,7 +1621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1628,23 +1645,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C21" sqref="C21:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1672,7 +1689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1686,7 +1703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1700,7 +1717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1714,7 +1731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1728,7 +1745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1742,7 +1759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1756,7 +1773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1770,7 +1787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1784,7 +1801,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1798,7 +1815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1812,7 +1829,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1826,7 +1843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -1840,7 +1857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1854,7 +1871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>15</v>
       </c>
@@ -1868,7 +1885,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>16</v>
       </c>
@@ -1882,7 +1899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -1896,7 +1913,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>18</v>
       </c>
@@ -1910,7 +1927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -1934,23 +1951,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1978,7 +1995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1992,7 +2009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -2006,7 +2023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -2020,7 +2037,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -2034,7 +2051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -2058,23 +2075,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +2105,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -2102,7 +2119,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -2116,21 +2133,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -2144,7 +2161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -2158,35 +2175,35 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -2200,7 +2217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -2214,21 +2231,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>11</v>
       </c>

</xml_diff>